<commit_message>
fixes in output dict creation, improved annotations, protocol changes
</commit_message>
<xml_diff>
--- a/Output/Animal10.xlsx
+++ b/Output/Animal10.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>strength (raw)</t>
+          <t>strength (RMS)</t>
         </is>
       </c>
     </row>
@@ -467,16 +467,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12.4</v>
+        <v>14</v>
       </c>
       <c r="C2" t="n">
         <v>27.6</v>
       </c>
       <c r="D2" t="n">
-        <v>15.2</v>
+        <v>13.6</v>
       </c>
       <c r="E2" t="n">
-        <v>151.6</v>
+        <v>76.2</v>
       </c>
     </row>
     <row r="3">
@@ -486,16 +486,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>14.5</v>
       </c>
       <c r="C3" t="n">
         <v>31</v>
       </c>
       <c r="D3" t="n">
-        <v>18</v>
+        <v>16.5</v>
       </c>
       <c r="E3" t="n">
-        <v>147.25</v>
+        <v>79.5</v>
       </c>
     </row>
     <row r="4">
@@ -505,16 +505,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12.8</v>
+        <v>14</v>
       </c>
       <c r="C4" t="n">
         <v>30.8</v>
       </c>
       <c r="D4" t="n">
-        <v>18</v>
+        <v>16.8</v>
       </c>
       <c r="E4" t="n">
-        <v>150.8</v>
+        <v>75.2</v>
       </c>
     </row>
     <row r="5">
@@ -524,16 +524,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>13.2</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
         <v>35.2</v>
       </c>
       <c r="D5" t="n">
-        <v>22</v>
+        <v>21.2</v>
       </c>
       <c r="E5" t="n">
-        <v>154.8</v>
+        <v>77.8</v>
       </c>
     </row>
     <row r="6">
@@ -543,16 +543,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>12.8</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
         <v>30.4</v>
       </c>
       <c r="D6" t="n">
-        <v>17.6</v>
+        <v>16.4</v>
       </c>
       <c r="E6" t="n">
-        <v>137.2</v>
+        <v>73.2</v>
       </c>
     </row>
     <row r="7">
@@ -562,16 +562,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>12.8</v>
+        <v>14.4</v>
       </c>
       <c r="C7" t="n">
         <v>28.4</v>
       </c>
       <c r="D7" t="n">
-        <v>15.6</v>
+        <v>14</v>
       </c>
       <c r="E7" t="n">
-        <v>126.6</v>
+        <v>67.2</v>
       </c>
     </row>
     <row r="8">
@@ -581,16 +581,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>12.4</v>
+        <v>14</v>
       </c>
       <c r="C8" t="n">
         <v>30.4</v>
       </c>
       <c r="D8" t="n">
-        <v>18</v>
+        <v>16.4</v>
       </c>
       <c r="E8" t="n">
-        <v>140.2</v>
+        <v>72.59999999999999</v>
       </c>
     </row>
     <row r="9">
@@ -600,16 +600,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>12.4</v>
+        <v>14</v>
       </c>
       <c r="C9" t="n">
         <v>32.8</v>
       </c>
       <c r="D9" t="n">
-        <v>20.4</v>
+        <v>18.8</v>
       </c>
       <c r="E9" t="n">
-        <v>141.8</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10">
@@ -619,16 +619,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>12.8</v>
       </c>
       <c r="C10" t="n">
         <v>32.4</v>
       </c>
       <c r="D10" t="n">
-        <v>20.4</v>
+        <v>19.6</v>
       </c>
       <c r="E10" t="n">
-        <v>162.6</v>
+        <v>77.40000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -638,16 +638,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C11" t="n">
         <v>45.6</v>
       </c>
       <c r="D11" t="n">
-        <v>33.6</v>
+        <v>31.6</v>
       </c>
       <c r="E11" t="n">
-        <v>136.2</v>
+        <v>71.8</v>
       </c>
     </row>
     <row r="12">
@@ -657,16 +657,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>13.6</v>
+        <v>14.4</v>
       </c>
       <c r="C12" t="n">
         <v>31.2</v>
       </c>
       <c r="D12" t="n">
-        <v>17.6</v>
+        <v>16.8</v>
       </c>
       <c r="E12" t="n">
-        <v>126</v>
+        <v>66.8</v>
       </c>
     </row>
     <row r="13">
@@ -676,16 +676,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>13.6</v>
+        <v>14</v>
       </c>
       <c r="C13" t="n">
         <v>31.6</v>
       </c>
       <c r="D13" t="n">
-        <v>18</v>
+        <v>17.6</v>
       </c>
       <c r="E13" t="n">
-        <v>139.8</v>
+        <v>71.40000000000001</v>
       </c>
     </row>
     <row r="14">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>12.67</v>
+        <v>13.33</v>
       </c>
       <c r="C14" t="n">
         <v>30.67</v>
       </c>
       <c r="D14" t="n">
-        <v>18</v>
+        <v>17.33</v>
       </c>
       <c r="E14" t="n">
-        <v>154.33</v>
+        <v>73.67</v>
       </c>
     </row>
     <row r="15">
@@ -714,16 +714,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" t="n">
         <v>31</v>
       </c>
       <c r="D15" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" t="n">
-        <v>131.5</v>
+        <v>66.25</v>
       </c>
     </row>
     <row r="16">
@@ -733,16 +733,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>12.4</v>
+        <v>14</v>
       </c>
       <c r="C16" t="n">
         <v>34.4</v>
       </c>
       <c r="D16" t="n">
-        <v>22</v>
+        <v>20.4</v>
       </c>
       <c r="E16" t="n">
-        <v>156.2</v>
+        <v>78.8</v>
       </c>
     </row>
     <row r="17">
@@ -752,16 +752,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>12.4</v>
+        <v>13.6</v>
       </c>
       <c r="C17" t="n">
         <v>34.4</v>
       </c>
       <c r="D17" t="n">
-        <v>22</v>
+        <v>20.8</v>
       </c>
       <c r="E17" t="n">
-        <v>161.6</v>
+        <v>82.2</v>
       </c>
     </row>
     <row r="18">
@@ -771,16 +771,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>14</v>
+        <v>15.2</v>
       </c>
       <c r="C18" t="n">
         <v>31.2</v>
       </c>
       <c r="D18" t="n">
-        <v>17.2</v>
+        <v>16</v>
       </c>
       <c r="E18" t="n">
-        <v>120.6</v>
+        <v>69.59999999999999</v>
       </c>
     </row>
     <row r="19">
@@ -790,16 +790,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12.4</v>
+        <v>12.8</v>
       </c>
       <c r="C19" t="n">
         <v>30.8</v>
       </c>
       <c r="D19" t="n">
-        <v>18.4</v>
+        <v>18</v>
       </c>
       <c r="E19" t="n">
-        <v>150.2</v>
+        <v>72.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>